<commit_message>
Planes de cuentas arreglados
</commit_message>
<xml_diff>
--- a/src/plantillas/pruebas.xlsx
+++ b/src/plantillas/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pruebas con js\src\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FD5A17-B083-4419-8482-4F3F34D9B4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F8443C-C2A6-4CCA-A68B-B2B4116DFC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,8 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +357,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,17 +368,17 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>